<commit_message>
MPS added, DGSA includes SOM
</commit_message>
<xml_diff>
--- a/docs/DistributionTable.xlsx
+++ b/docs/DistributionTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23970" windowHeight="7830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="heterogenous" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Parameter Name (code)</t>
   </si>
@@ -108,6 +108,36 @@
   </si>
   <si>
     <t>[0 Exponential, 1 Gaussian]</t>
+  </si>
+  <si>
+    <t>MPS</t>
+  </si>
+  <si>
+    <t>TI_rivlen</t>
+  </si>
+  <si>
+    <t>TI_rivwidth</t>
+  </si>
+  <si>
+    <t>500m-2km</t>
+  </si>
+  <si>
+    <t>TI_sinuosity</t>
+  </si>
+  <si>
+    <t>27km of Salinas Valley = 37km of river</t>
+  </si>
+  <si>
+    <t>Quick measurements from N Sal Valley</t>
+  </si>
+  <si>
+    <t>2-4km</t>
+  </si>
+  <si>
+    <t>TI_rivwavelength</t>
+  </si>
+  <si>
+    <t>continuous</t>
   </si>
 </sst>
 </file>
@@ -434,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,6 +601,52 @@
         <v>22</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>1.341</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>